<commit_message>
A ce stade less tables de la base de données sont en conformité avec PEP8 et les dates sont au format julien
</commit_message>
<xml_diff>
--- a/sources/lexiques.xlsx
+++ b/sources/lexiques.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Yvon\AAAAA-Mes-donnees\Mes-developpements\Python_tous_mes_tutoriels\projet_rgd_pas_a_pas\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2B9F92-9151-449F-8DDE-306481FBA761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E287E33-35BB-4980-B025-03B74F110AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F_definition_cles_repartitions" sheetId="2" r:id="rId1"/>
@@ -21,9 +21,11 @@
     <sheet name="F_liste_groupes" sheetId="7" r:id="rId6"/>
     <sheet name="F_liste_groupe_a_etudier" sheetId="8" r:id="rId7"/>
     <sheet name="Noms_champs" sheetId="10" r:id="rId8"/>
+    <sheet name="Règles de nommage (PEP8)" sheetId="11" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="Agregation_2015_a_2019">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">'Règles de nommage (PEP8)'!$A$1:$E$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="465">
   <si>
     <t>E</t>
   </si>
@@ -1351,6 +1353,798 @@
   </si>
   <si>
     <t>recurrent</t>
+  </si>
+  <si>
+    <t>Noms de variables et fonctions</t>
+  </si>
+  <si>
+    <r>
+      <t>minuscules</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, avec des mots séparés par des underscores (snake_case)</t>
+    </r>
+  </si>
+  <si>
+    <t>Noms de classes</t>
+  </si>
+  <si>
+    <r>
+      <t>CamelCase</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (première lettre de chaque mot en majuscule, sans underscore)</t>
+    </r>
+  </si>
+  <si>
+    <t>Constantes</t>
+  </si>
+  <si>
+    <r>
+      <t>MAJUSCULES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, avec underscores</t>
+    </r>
+  </si>
+  <si>
+    <t>Modules et packages</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">noms </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>courts, en minuscules</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, éventuellement avec underscore si nécessaire</t>
+    </r>
+  </si>
+  <si>
+    <t>Attributs privés / internes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Préfixe par un </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">underscore </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (indique que ce n’est pas destiné à être utilisé en dehors du module/classe)</t>
+    </r>
+  </si>
+  <si>
+    <t>Variables spéciales (réservées par Python)</t>
+  </si>
+  <si>
+    <r>
+      <t>Double underscore avant et après (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>__dunder__</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) → utilisés par Python pour ses propres méthodes spéciales</t>
+    </r>
+  </si>
+  <si>
+    <t>Longueur et lisibilité</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Utiliser des noms </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>significatifs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, pas de lettres isolées sauf pour les boucles très courtes :</t>
+    </r>
+  </si>
+  <si>
+    <t>class InvoiceLine(Base): ...</t>
+  </si>
+  <si>
+    <r>
+      <t>Classe Python (ORM)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>CamelCase</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Table SQL / tablename</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>snake_case</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (recommandé : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>singulier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, ex. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>invoice_line</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(Singulier vs pluriel : cohérence ; je recommande </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>singulier</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> — une ligne = un enregistrement.)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Colonnes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>snake_case</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> en </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>minuscules</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, ex. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>created_at</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>amount_eur</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (colonne courte et standard) → </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>id</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>FK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;referenced_entity&gt;_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, ex. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>user_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>invoice_id</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Table d'association (many-to-many)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>entity1_entity2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> — choisissez un ordre déterministe (ex. alphabetique) ou votre préférence (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>group_user</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ou </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>user_group</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) — </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>soyez consistant</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Index</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>ix_&lt;table&gt;_&lt;column1&gt;[_&lt;column2&gt;]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Unique</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>uq_&lt;table&gt;_&lt;column&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ForeignKey constraint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>fk_&lt;table&gt;_&lt;column&gt;_&lt;referred_table&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Primary key constraint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>pk_&lt;table&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>View</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>view_&lt;name&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ou </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>vw_&lt;name&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (choix de projet)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Séquence (Postgres)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>&lt;table&gt;_&lt;column&gt;_seq</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (si utilisée)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Longueur</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : évitez des noms &gt; ~63 caractères (Postgres limite à 63 ; Oracle ~30).</t>
+    </r>
+  </si>
+  <si>
+    <t>Règles de nommage</t>
+  </si>
+  <si>
+    <t>Récapitulatif rapide bases de données</t>
   </si>
 </sst>
 </file>
@@ -1362,7 +2156,7 @@
     <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="166" formatCode="d/m/yy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1383,12 +2177,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -1397,6 +2185,53 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="18"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1433,39 +2268,39 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1485,6 +2320,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1775,7 +2625,7 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -5924,4 +6774,233 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46DB1BB2-6ACE-438E-8C42-3EC7DFCD420B}">
+  <dimension ref="A1:E43"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="2" width="1.53515625" customWidth="1"/>
+    <col min="3" max="3" width="66.07421875" customWidth="1"/>
+    <col min="4" max="4" width="1.69140625" customWidth="1"/>
+    <col min="5" max="5" width="89.53515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B3" s="24" t="s">
+        <v>434</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="E3" s="24" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B5" s="24" t="s">
+        <v>436</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="E5" s="24" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B7" s="24" t="s">
+        <v>438</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="E7" s="24" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B9" s="24" t="s">
+        <v>440</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="E9" s="23" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B11" s="24" t="s">
+        <v>442</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="E11" s="23" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B13" s="24" t="s">
+        <v>444</v>
+      </c>
+      <c r="C13" s="24"/>
+      <c r="E13" s="23" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B15" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="C15" s="24"/>
+      <c r="E15" s="23" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="23.15" x14ac:dyDescent="0.4">
+      <c r="B17" s="27" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C18" s="23"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C19" s="24" t="s">
+        <v>449</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C20" s="23"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C21" s="24" t="s">
+        <v>450</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C22" s="23"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C23" s="24" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C24" s="23"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C25" s="24" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C26" s="23"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C27" s="24" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C28" s="23"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C29" s="24" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C30" s="23"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C31" s="24" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C32" s="23"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C33" s="24" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C34" s="23"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C35" s="24" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C36" s="23"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C37" s="24" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C38" s="23"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C39" s="24" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C40" s="23"/>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C41" s="24" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C42" s="23"/>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.4">
+      <c r="C43" s="24" t="s">
+        <v>462</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.27559055118110237" bottom="0.23622047244094491" header="0.15748031496062992" footer="0.15748031496062992"/>
+  <pageSetup paperSize="9" scale="80" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Module "Actualisation des données" fonctionne
</commit_message>
<xml_diff>
--- a/sources/lexiques.xlsx
+++ b/sources/lexiques.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Yvon\AAAAA-Mes-donnees\Mes-developpements\Python_tous_mes_tutoriels\projet_rgd_pas_a_pas\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E287E33-35BB-4980-B025-03B74F110AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17196AA-B6CD-4FF2-9420-3DA5C11538FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F_definition_cles_repartitions" sheetId="2" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="F_liste_groupe_a_etudier" sheetId="8" r:id="rId7"/>
     <sheet name="Noms_champs" sheetId="10" r:id="rId8"/>
     <sheet name="Règles de nommage (PEP8)" sheetId="11" r:id="rId9"/>
+    <sheet name="Classe vs Table" sheetId="12" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="Agregation_2015_a_2019">#REF!</definedName>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="483">
   <si>
     <t>E</t>
   </si>
@@ -2145,6 +2146,65 @@
   </si>
   <si>
     <t>Récapitulatif rapide bases de données</t>
+  </si>
+  <si>
+    <t>Utilisateur.__table__.c.nom (colonne brute SQL)</t>
+  </si>
+  <si>
+    <t>Utilisateur.nom (colonne ORM dans une requête)</t>
+  </si>
+  <si>
+    <t>Accès colonnes</t>
+  </si>
+  <si>
+    <t>stmt = Utilisateur.__table__.delete().where(Utilisateur.__table__.c.id &gt; 10)_x000D_
+session.execute(stmt)</t>
+  </si>
+  <si>
+    <t>session.execute(delete(Utilisateur).where(Utilisateur.id &gt; 10))</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>stmt = Utilisateur.__table__.update().where(Utilisateur.__table__.c.id==1).values(prenom='Bob')_x000D_
+session.execute(stmt)</t>
+  </si>
+  <si>
+    <t>session.execute(update(Utilisateur).where(Utilisateur.id==1).values(prenom='Bob'))</t>
+  </si>
+  <si>
+    <t>UPDATE</t>
+  </si>
+  <si>
+    <t>stmt = Utilisateur.__table__.insert().values(nom='Dupont', prenom='Alice')_x000D_
+session.execute(stmt)</t>
+  </si>
+  <si>
+    <t>u = Utilisateur(nom='Dupont', prenom='Alice')_x000D_
+session.add(u)_x000D_
+session.commit()</t>
+  </si>
+  <si>
+    <t>INSERT</t>
+  </si>
+  <si>
+    <t>session.execute(select(Utilisateur.__table__).where(Utilisateur.__table__.c.nom == 'Dupont'))</t>
+  </si>
+  <si>
+    <t>session.execute(select(Utilisateur).where(Utilisateur.nom == 'Dupont'))</t>
+  </si>
+  <si>
+    <t>SELECT</t>
+  </si>
+  <si>
+    <t>Avec Table (Core)</t>
+  </si>
+  <si>
+    <t>Avec Classe (ORM)</t>
+  </si>
+  <si>
+    <t>Action</t>
   </si>
 </sst>
 </file>
@@ -2237,7 +2297,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2253,6 +2313,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6666FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2275,7 +2347,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2336,6 +2408,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3345,6 +3421,93 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC9D70F-0DD0-4852-8227-16C3CCD3CB80}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="13.4609375" customWidth="1"/>
+    <col min="2" max="2" width="69.3046875" customWidth="1"/>
+    <col min="3" max="3" width="98.3046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="28" t="s">
+        <v>482</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>481</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" s="29" t="s">
+        <v>479</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>478</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3" t="s">
+        <v>475</v>
+      </c>
+      <c r="C3" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" s="29" t="s">
+        <v>473</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>472</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>470</v>
+      </c>
+      <c r="B5" t="s">
+        <v>469</v>
+      </c>
+      <c r="C5" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" s="29" t="s">
+        <v>467</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>466</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>465</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Feuil2"/>
@@ -6780,7 +6943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46DB1BB2-6ACE-438E-8C42-3EC7DFCD420B}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection sqref="A1:E43"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
L'étape "réinitialisation" de la BDD foncttionne
</commit_message>
<xml_diff>
--- a/sources/lexiques.xlsx
+++ b/sources/lexiques.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Yvon\AAAAA-Mes-donnees\Mes-developpements\Python_tous_mes_tutoriels\projet_rgd_pas_a_pas\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17196AA-B6CD-4FF2-9420-3DA5C11538FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E265AE0B-4D0A-41C1-89FD-82A9433E376D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F_definition_cles_repartitions" sheetId="2" r:id="rId1"/>
@@ -19,8 +19,8 @@
     <sheet name="F_lexique_rub" sheetId="5" r:id="rId4"/>
     <sheet name="F_lexique_typ" sheetId="6" r:id="rId5"/>
     <sheet name="F_liste_groupes" sheetId="7" r:id="rId6"/>
-    <sheet name="F_liste_groupe_a_etudier" sheetId="8" r:id="rId7"/>
-    <sheet name="Noms_champs" sheetId="10" r:id="rId8"/>
+    <sheet name="F_liste_groupes_a_etudier" sheetId="8" r:id="rId7"/>
+    <sheet name="Nom champs" sheetId="10" r:id="rId8"/>
     <sheet name="Règles de nommage (PEP8)" sheetId="11" r:id="rId9"/>
     <sheet name="Classe vs Table" sheetId="12" r:id="rId10"/>
   </sheets>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="491">
   <si>
     <t>E</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Village</t>
   </si>
   <si>
-    <t>ASL</t>
-  </si>
-  <si>
     <t>ER</t>
   </si>
   <si>
@@ -141,12 +138,6 @@
     <t>Village/Special</t>
   </si>
   <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>Verif</t>
-  </si>
-  <si>
     <t>ACC_2001</t>
   </si>
   <si>
@@ -1239,9 +1230,6 @@
     <t>Nom du fournisseur</t>
   </si>
   <si>
-    <t>montant_a_repartir</t>
-  </si>
-  <si>
     <t>Montant à repartir</t>
   </si>
   <si>
@@ -1327,9 +1315,6 @@
   </si>
   <si>
     <t>batrub</t>
-  </si>
-  <si>
-    <t>batrub_tit</t>
   </si>
   <si>
     <t>entites</t>
@@ -2205,6 +2190,45 @@
   </si>
   <si>
     <t>Action</t>
+  </si>
+  <si>
+    <t>batrub_tit_yp</t>
+  </si>
+  <si>
+    <t>bat_tit_yp</t>
+  </si>
+  <si>
+    <t>rub_tit_yp</t>
+  </si>
+  <si>
+    <t>typ_tit_yp</t>
+  </si>
+  <si>
+    <t>montant</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>asl</t>
+  </si>
+  <si>
+    <t>er</t>
+  </si>
+  <si>
+    <t>erg</t>
+  </si>
+  <si>
+    <t>verif</t>
   </si>
 </sst>
 </file>
@@ -2701,7 +2725,9 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -2711,36 +2737,36 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>0</v>
+        <v>483</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>1</v>
+        <v>484</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>2</v>
+        <v>485</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>29</v>
+        <v>486</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>4</v>
+        <v>487</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>5</v>
+        <v>488</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>6</v>
+        <v>489</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>30</v>
+        <v>490</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="13">
         <v>0.24099999999999999</v>
@@ -2769,7 +2795,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="13">
         <v>0.45400000000000001</v>
@@ -2798,7 +2824,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="13">
         <v>0.34</v>
@@ -2827,7 +2853,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="13">
         <v>0.16</v>
@@ -2856,7 +2882,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="13">
         <v>0.34300000000000003</v>
@@ -2885,7 +2911,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="13">
         <v>0.33300000000000002</v>
@@ -2914,7 +2940,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="13">
         <v>0.38200000000000001</v>
@@ -2943,7 +2969,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="13">
         <v>0</v>
@@ -2972,7 +2998,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="13">
         <v>0</v>
@@ -3001,7 +3027,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="13">
         <v>0</v>
@@ -3030,7 +3056,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="13">
         <v>0</v>
@@ -3059,7 +3085,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="13">
         <v>1</v>
@@ -3088,7 +3114,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="13">
         <v>1</v>
@@ -3117,7 +3143,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="13">
         <v>0</v>
@@ -3146,7 +3172,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="13">
         <v>0</v>
@@ -3175,7 +3201,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="13">
         <v>0</v>
@@ -3204,7 +3230,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="13">
         <v>1</v>
@@ -3233,7 +3259,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="13">
         <v>0</v>
@@ -3262,7 +3288,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="13">
         <v>1</v>
@@ -3291,7 +3317,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="13">
         <v>0</v>
@@ -3320,7 +3346,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="13">
         <v>0</v>
@@ -3349,7 +3375,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B23" s="13">
         <v>0.27300000000000002</v>
@@ -3378,7 +3404,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B24" s="13">
         <v>0.25700000000000001</v>
@@ -3425,7 +3451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC9D70F-0DD0-4852-8227-16C3CCD3CB80}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:C6"/>
     </sheetView>
   </sheetViews>
@@ -3438,68 +3464,68 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="28" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="29" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="B3" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="C3" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="29" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="B5" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="C5" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="29" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -3527,19 +3553,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" s="17" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>425</v>
+        <v>478</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -3547,13 +3573,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>3</v>
@@ -3567,19 +3593,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -3587,19 +3613,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -3607,19 +3633,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -3627,19 +3653,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -3647,13 +3673,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>3</v>
@@ -3667,19 +3693,19 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -3687,19 +3713,19 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -3707,19 +3733,19 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -3727,13 +3753,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>3</v>
@@ -3747,19 +3773,19 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>1</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -3767,19 +3793,19 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>1</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -3787,19 +3813,19 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -3807,19 +3833,19 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -3827,19 +3853,19 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>1</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -3847,19 +3873,19 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17" s="11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -3867,19 +3893,19 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>1</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -3887,19 +3913,19 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A19" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -3907,19 +3933,19 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A20" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -3927,19 +3953,19 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A21" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -3947,19 +3973,19 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A22" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>0</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -3967,19 +3993,19 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>0</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -3987,19 +4013,19 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A24" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -4007,19 +4033,19 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A25" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -4047,10 +4073,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" s="18" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>421</v>
+        <v>479</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -4061,10 +4087,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -4075,10 +4101,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -4089,10 +4115,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -4103,10 +4129,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -4117,10 +4143,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -4131,10 +4157,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -4145,10 +4171,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -4159,10 +4185,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -4173,10 +4199,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -4187,10 +4213,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -4201,10 +4227,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" s="10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -4215,10 +4241,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" s="10" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -4229,10 +4255,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" s="10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -4243,10 +4269,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" s="10" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -4366,7 +4392,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4377,114 +4403,114 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="19" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>422</v>
+        <v>480</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" s="9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" s="9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" s="9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.4">
@@ -4542,7 +4568,7 @@
   <dimension ref="A1:H125"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4553,13 +4579,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" s="20" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>423</v>
+        <v>481</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -4569,10 +4595,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C2" s="8" t="b">
         <v>0</v>
@@ -4585,10 +4611,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C3" s="8" t="b">
         <v>0</v>
@@ -4601,10 +4627,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="7" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C4" s="8" t="b">
         <v>0</v>
@@ -4617,10 +4643,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C5" s="8" t="b">
         <v>0</v>
@@ -4633,10 +4659,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C6" s="8" t="b">
         <v>0</v>
@@ -4649,10 +4675,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C7" s="8" t="b">
         <v>0</v>
@@ -4665,10 +4691,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C8" s="8" t="b">
         <v>0</v>
@@ -4681,10 +4707,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C9" s="8" t="b">
         <v>0</v>
@@ -4697,10 +4723,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C10" s="8" t="b">
         <v>0</v>
@@ -4713,10 +4739,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C11" s="8" t="b">
         <v>0</v>
@@ -4729,10 +4755,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C12" s="8" t="b">
         <v>0</v>
@@ -4745,10 +4771,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C13" s="8" t="b">
         <v>0</v>
@@ -4761,10 +4787,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C14" s="8" t="b">
         <v>1</v>
@@ -4777,10 +4803,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C15" s="8" t="b">
         <v>1</v>
@@ -4793,10 +4819,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" s="7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C16" s="8" t="b">
         <v>0</v>
@@ -4809,10 +4835,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C17" s="8" t="b">
         <v>0</v>
@@ -4825,10 +4851,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C18" s="8" t="b">
         <v>0</v>
@@ -4841,10 +4867,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A19" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C19" s="8" t="b">
         <v>0</v>
@@ -4857,10 +4883,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A20" s="7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C20" s="8" t="b">
         <v>0</v>
@@ -4873,10 +4899,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A21" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C21" s="8" t="b">
         <v>0</v>
@@ -4889,10 +4915,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A22" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C22" s="8" t="b">
         <v>1</v>
@@ -4905,10 +4931,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C23" s="8" t="b">
         <v>0</v>
@@ -4921,10 +4947,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A24" s="7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C24" s="8" t="b">
         <v>0</v>
@@ -4937,10 +4963,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A25" s="7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C25" s="8" t="b">
         <v>0</v>
@@ -4953,10 +4979,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A26" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C26" s="8" t="b">
         <v>0</v>
@@ -4964,10 +4990,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A27" s="7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C27" s="8" t="b">
         <v>0</v>
@@ -4975,10 +5001,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A28" s="7" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C28" s="8" t="b">
         <v>0</v>
@@ -4986,10 +5012,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A29" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C29" s="8" t="b">
         <v>0</v>
@@ -4997,10 +5023,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A30" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C30" s="8" t="b">
         <v>0</v>
@@ -5008,10 +5034,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A31" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C31" s="8" t="b">
         <v>0</v>
@@ -5019,10 +5045,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A32" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C32" s="8" t="b">
         <v>0</v>
@@ -5030,10 +5056,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C33" s="8" t="b">
         <v>0</v>
@@ -5041,10 +5067,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A34" s="7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C34" s="8" t="b">
         <v>0</v>
@@ -5052,10 +5078,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A35" s="7" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C35" s="8" t="b">
         <v>0</v>
@@ -5063,10 +5089,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A36" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C36" s="8" t="b">
         <v>0</v>
@@ -5074,10 +5100,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C37" s="8" t="b">
         <v>0</v>
@@ -5085,10 +5111,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A38" s="7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C38" s="8" t="b">
         <v>0</v>
@@ -5096,10 +5122,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A39" s="7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C39" s="8" t="b">
         <v>0</v>
@@ -5107,10 +5133,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A40" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C40" s="8" t="b">
         <v>0</v>
@@ -5118,10 +5144,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A41" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C41" s="8" t="b">
         <v>0</v>
@@ -5129,10 +5155,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A42" s="7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C42" s="8" t="b">
         <v>0</v>
@@ -5140,10 +5166,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A43" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C43" s="8" t="b">
         <v>0</v>
@@ -5151,10 +5177,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A44" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C44" s="8" t="b">
         <v>0</v>
@@ -5162,10 +5188,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A45" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C45" s="8" t="b">
         <v>0</v>
@@ -5173,10 +5199,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A46" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C46" s="8" t="b">
         <v>0</v>
@@ -5184,10 +5210,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A47" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C47" s="8" t="b">
         <v>0</v>
@@ -5195,10 +5221,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A48" s="7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C48" s="8" t="b">
         <v>0</v>
@@ -5206,10 +5232,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A49" s="7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C49" s="8" t="b">
         <v>0</v>
@@ -5217,10 +5243,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A50" s="7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C50" s="8" t="b">
         <v>0</v>
@@ -5228,10 +5254,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A51" s="7" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C51" s="8" t="b">
         <v>0</v>
@@ -5239,10 +5265,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A52" s="7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C52" s="8" t="b">
         <v>0</v>
@@ -5250,10 +5276,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A53" s="7" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C53" s="8" t="b">
         <v>0</v>
@@ -5261,10 +5287,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A54" s="7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C54" s="8" t="b">
         <v>0</v>
@@ -5272,10 +5298,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A55" s="7" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C55" s="8" t="b">
         <v>0</v>
@@ -5283,10 +5309,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A56" s="7" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C56" s="8" t="b">
         <v>0</v>
@@ -5294,10 +5320,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A57" s="7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C57" s="8" t="b">
         <v>0</v>
@@ -5305,10 +5331,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A58" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C58" s="8" t="b">
         <v>0</v>
@@ -5316,10 +5342,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A59" s="7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C59" s="8" t="b">
         <v>1</v>
@@ -5327,10 +5353,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A60" s="7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C60" s="8" t="b">
         <v>0</v>
@@ -5338,10 +5364,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A61" s="7" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C61" s="8" t="b">
         <v>0</v>
@@ -5349,10 +5375,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A62" s="7" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C62" s="8" t="b">
         <v>1</v>
@@ -5360,10 +5386,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A63" s="7" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C63" s="8" t="b">
         <v>0</v>
@@ -5371,10 +5397,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A64" s="7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C64" s="8" t="b">
         <v>0</v>
@@ -5382,10 +5408,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A65" s="7" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C65" s="8" t="b">
         <v>0</v>
@@ -5393,10 +5419,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A66" s="7" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C66" s="8" t="b">
         <v>0</v>
@@ -5404,10 +5430,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A67" s="7" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C67" s="8" t="b">
         <v>0</v>
@@ -5415,10 +5441,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A68" s="7" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C68" s="8" t="b">
         <v>0</v>
@@ -5426,10 +5452,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A69" s="7" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C69" s="8" t="b">
         <v>0</v>
@@ -5437,10 +5463,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A70" s="7" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C70" s="8" t="b">
         <v>0</v>
@@ -5448,10 +5474,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A71" s="7" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C71" s="8" t="b">
         <v>0</v>
@@ -5459,10 +5485,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A72" s="7" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C72" s="8" t="b">
         <v>0</v>
@@ -5470,10 +5496,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A73" s="7" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C73" s="8" t="b">
         <v>0</v>
@@ -5481,10 +5507,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A74" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C74" s="8" t="b">
         <v>0</v>
@@ -5492,10 +5518,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A75" s="7" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C75" s="8" t="b">
         <v>0</v>
@@ -5503,10 +5529,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A76" s="7" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C76" s="8" t="b">
         <v>0</v>
@@ -5514,10 +5540,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A77" s="7" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C77" s="8" t="b">
         <v>0</v>
@@ -5525,10 +5551,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A78" s="7" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C78" s="8" t="b">
         <v>0</v>
@@ -5536,10 +5562,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A79" s="7" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C79" s="8" t="b">
         <v>0</v>
@@ -5547,10 +5573,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A80" s="7" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C80" s="8" t="b">
         <v>0</v>
@@ -5558,10 +5584,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A81" s="7" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C81" s="8" t="b">
         <v>0</v>
@@ -5569,10 +5595,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A82" s="7" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C82" s="8" t="b">
         <v>0</v>
@@ -5580,10 +5606,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A83" s="7" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C83" s="8" t="b">
         <v>0</v>
@@ -5591,10 +5617,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A84" s="7" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C84" s="8" t="b">
         <v>0</v>
@@ -5602,10 +5628,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A85" s="7" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C85" s="8" t="b">
         <v>0</v>
@@ -5613,10 +5639,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A86" s="7" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C86" s="8" t="b">
         <v>0</v>
@@ -5624,10 +5650,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A87" s="7" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C87" s="8" t="b">
         <v>0</v>
@@ -5635,10 +5661,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A88" s="7" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C88" s="8" t="b">
         <v>0</v>
@@ -5646,10 +5672,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A89" s="7" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C89" s="8" t="b">
         <v>0</v>
@@ -5657,10 +5683,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A90" s="7" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C90" s="8" t="b">
         <v>0</v>
@@ -5668,10 +5694,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A91" s="7" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C91" s="8" t="b">
         <v>0</v>
@@ -5679,10 +5705,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A92" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C92" s="8" t="b">
         <v>0</v>
@@ -5690,10 +5716,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A93" s="7" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C93" s="8" t="b">
         <v>0</v>
@@ -5701,10 +5727,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A94" s="7" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C94" s="8" t="b">
         <v>0</v>
@@ -5712,10 +5738,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A95" s="7" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C95" s="8" t="b">
         <v>0</v>
@@ -5723,10 +5749,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A96" s="7" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C96" s="8" t="b">
         <v>0</v>
@@ -5734,10 +5760,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A97" s="7" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C97" s="8" t="b">
         <v>0</v>
@@ -5745,10 +5771,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A98" s="7" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C98" s="8" t="b">
         <v>0</v>
@@ -5756,10 +5782,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A99" s="7" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C99" s="8" t="b">
         <v>0</v>
@@ -5767,10 +5793,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A100" s="7" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C100" s="8" t="b">
         <v>0</v>
@@ -5778,10 +5804,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A101" s="7" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C101" s="8" t="b">
         <v>0</v>
@@ -5789,10 +5815,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A102" s="7" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C102" s="8" t="b">
         <v>0</v>
@@ -5800,10 +5826,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A103" s="7" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C103" s="8" t="b">
         <v>1</v>
@@ -5811,10 +5837,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A104" s="7" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C104" s="8" t="b">
         <v>0</v>
@@ -5822,10 +5848,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A105" s="7" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C105" s="8" t="b">
         <v>0</v>
@@ -5833,10 +5859,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A106" s="7" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C106" s="8" t="b">
         <v>0</v>
@@ -5844,10 +5870,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A107" s="7" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C107" s="8" t="b">
         <v>0</v>
@@ -5855,10 +5881,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A108" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C108" s="8" t="b">
         <v>0</v>
@@ -5866,10 +5892,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A109" s="7" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C109" s="8" t="b">
         <v>0</v>
@@ -5877,10 +5903,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A110" s="7" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C110" s="8" t="b">
         <v>0</v>
@@ -5888,10 +5914,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A111" s="7" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C111" s="8" t="b">
         <v>0</v>
@@ -5899,10 +5925,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A112" s="7" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C112" s="8" t="b">
         <v>0</v>
@@ -5910,10 +5936,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A113" s="7" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C113" s="8" t="b">
         <v>0</v>
@@ -5921,10 +5947,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A114" s="7" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C114" s="8" t="b">
         <v>0</v>
@@ -5932,10 +5958,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A115" s="7" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C115" s="8" t="b">
         <v>0</v>
@@ -5943,10 +5969,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A116" s="7" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C116" s="8" t="b">
         <v>0</v>
@@ -5954,10 +5980,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A117" s="7" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C117" s="8" t="b">
         <v>0</v>
@@ -5965,10 +5991,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A118" s="7" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C118" s="8" t="b">
         <v>0</v>
@@ -5976,10 +6002,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A119" s="7" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C119" s="8" t="b">
         <v>0</v>
@@ -5987,10 +6013,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A120" s="7" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C120" s="8" t="b">
         <v>1</v>
@@ -5998,10 +6024,10 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A121" s="7" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C121" s="8" t="b">
         <v>0</v>
@@ -6009,10 +6035,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A122" s="7" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C122" s="8" t="b">
         <v>0</v>
@@ -6020,10 +6046,10 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A123" s="7" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C123" s="8" t="b">
         <v>0</v>
@@ -6060,10 +6086,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" s="21" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -6074,7 +6100,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B2" s="6">
         <v>0</v>
@@ -6088,7 +6114,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B3" s="6">
         <v>-1</v>
@@ -6102,7 +6128,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B4" s="6">
         <v>0</v>
@@ -6116,7 +6142,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B5" s="6">
         <v>0</v>
@@ -6130,7 +6156,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B6" s="6">
         <v>-1</v>
@@ -6144,7 +6170,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B7" s="6">
         <v>-1</v>
@@ -6158,7 +6184,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B8" s="6">
         <v>0</v>
@@ -6172,7 +6198,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B9" s="6">
         <v>0</v>
@@ -6186,7 +6212,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B10" s="6">
         <v>-1</v>
@@ -6200,7 +6226,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B11" s="6">
         <v>-1</v>
@@ -6214,7 +6240,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B12" s="6">
         <v>0</v>
@@ -6228,7 +6254,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B13" s="6">
         <v>-1</v>
@@ -6242,7 +6268,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B14" s="6">
         <v>0</v>
@@ -6256,7 +6282,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B15" s="6">
         <v>-1</v>
@@ -6270,7 +6296,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B16" s="6">
         <v>0</v>
@@ -6284,7 +6310,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B17" s="6">
         <v>0</v>
@@ -6298,7 +6324,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18" s="5" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B18" s="6">
         <v>0</v>
@@ -6312,7 +6338,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A19" s="5" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B19" s="6">
         <v>0</v>
@@ -6326,7 +6352,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A20" s="5" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B20" s="6">
         <v>0</v>
@@ -6340,7 +6366,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A21" s="5" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B21" s="6">
         <v>0</v>
@@ -6354,7 +6380,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A22" s="5" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B22" s="6">
         <v>0</v>
@@ -6368,7 +6394,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23" s="5" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B23" s="6">
         <v>0</v>
@@ -6382,7 +6408,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A24" s="5" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B24" s="6">
         <v>0</v>
@@ -6396,7 +6422,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A25" s="5" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B25" s="6">
         <v>-1</v>
@@ -6410,7 +6436,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B26" s="6">
         <v>-1</v>
@@ -6418,7 +6444,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A27" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B27" s="6">
         <v>-1</v>
@@ -6426,7 +6452,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A28" s="5" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B28" s="6">
         <v>-1</v>
@@ -6434,7 +6460,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A29" s="5" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="B29" s="6">
         <v>-1</v>
@@ -6442,7 +6468,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A30" s="5" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B30" s="6">
         <v>0</v>
@@ -6450,7 +6476,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A31" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B31" s="6">
         <v>-1</v>
@@ -6458,7 +6484,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B32" s="6">
         <v>0</v>
@@ -6466,7 +6492,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A33" s="5" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B33" s="6">
         <v>0</v>
@@ -6482,8 +6508,8 @@
   <sheetPr codeName="Feuil7"/>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L44" sqref="L44"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -6493,7 +6519,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" s="22" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6505,7 +6531,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -6517,7 +6543,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -6529,7 +6555,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -6541,7 +6567,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -6553,7 +6579,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -6565,7 +6591,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -6577,7 +6603,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -6589,7 +6615,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -6601,7 +6627,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -6613,7 +6639,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -6625,7 +6651,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -6637,7 +6663,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -6649,7 +6675,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -6661,7 +6687,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -6673,7 +6699,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -6685,7 +6711,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -6697,7 +6723,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -6789,7 +6815,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -6800,138 +6826,138 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="16" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="B2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B3" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="15" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B4" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="14" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B5" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B6" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B7" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B8" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B9" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="B10" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="B11" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B12" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="B13" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B14" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B15" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="B16" t="s">
-        <v>395</v>
+        <v>482</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="B17" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
   </sheetData>
@@ -6957,16 +6983,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B3" s="24" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="C3" s="24"/>
       <c r="E3" s="24" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
@@ -6975,11 +7001,11 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B5" s="24" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="C5" s="24"/>
       <c r="E5" s="24" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
@@ -6988,11 +7014,11 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B7" s="24" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="C7" s="24"/>
       <c r="E7" s="24" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
@@ -7001,11 +7027,11 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B9" s="24" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="C9" s="24"/>
       <c r="E9" s="23" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
@@ -7014,11 +7040,11 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B11" s="24" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="C11" s="24"/>
       <c r="E11" s="23" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
@@ -7027,11 +7053,11 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B13" s="24" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="C13" s="24"/>
       <c r="E13" s="23" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
@@ -7040,16 +7066,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B15" s="24" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="C15" s="24"/>
       <c r="E15" s="23" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="23.15" x14ac:dyDescent="0.4">
       <c r="B17" s="27" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.4">
@@ -7057,10 +7083,10 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C19" s="24" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.4">
@@ -7068,10 +7094,10 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C21" s="24" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.4">
@@ -7079,7 +7105,7 @@
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C23" s="24" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.4">
@@ -7087,7 +7113,7 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C25" s="24" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.4">
@@ -7095,7 +7121,7 @@
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C27" s="24" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.4">
@@ -7103,7 +7129,7 @@
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C29" s="24" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.4">
@@ -7111,7 +7137,7 @@
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.4">
       <c r="C31" s="24" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.4">
@@ -7119,7 +7145,7 @@
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C33" s="24" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.4">
@@ -7127,7 +7153,7 @@
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C35" s="24" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.4">
@@ -7135,7 +7161,7 @@
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C37" s="24" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.4">
@@ -7143,7 +7169,7 @@
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C39" s="24" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.4">
@@ -7151,7 +7177,7 @@
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C41" s="24" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.4">
@@ -7159,7 +7185,7 @@
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C43" s="24" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
L'étape reinitialiser_bdd (formule revue) fonctionne
</commit_message>
<xml_diff>
--- a/sources/lexiques.xlsx
+++ b/sources/lexiques.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Yvon\AAAAA-Mes-donnees\Mes-developpements\Python_tous_mes_tutoriels\projet_rgd_pas_a_pas\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E265AE0B-4D0A-41C1-89FD-82A9433E376D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B611D0F4-7DF4-4C3B-AD43-BC4CB0495122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F_definition_cles_repartitions" sheetId="2" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Nom champs" sheetId="10" r:id="rId8"/>
     <sheet name="Règles de nommage (PEP8)" sheetId="11" r:id="rId9"/>
     <sheet name="Classe vs Table" sheetId="12" r:id="rId10"/>
+    <sheet name="Processus" sheetId="13" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="Agregation_2015_a_2019">#REF!</definedName>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="554">
   <si>
     <t>E</t>
   </si>
@@ -2230,6 +2231,195 @@
   <si>
     <t>verif</t>
   </si>
+  <si>
+    <t>Initialisation</t>
+  </si>
+  <si>
+    <t>F_definition_cles_repartitions</t>
+  </si>
+  <si>
+    <t>lexiques.xls</t>
+  </si>
+  <si>
+    <t>F_lexique_bat</t>
+  </si>
+  <si>
+    <t>F_lexique_rub</t>
+  </si>
+  <si>
+    <t>F_liste_groupes</t>
+  </si>
+  <si>
+    <t>F_liste_groupes_a_etudier</t>
+  </si>
+  <si>
+    <t>F_roc_modifiee</t>
+  </si>
+  <si>
+    <t>F_lexique_typ</t>
+  </si>
+  <si>
+    <t>F_parametres</t>
+  </si>
+  <si>
+    <t>F_agregation</t>
+  </si>
+  <si>
+    <t>Actualisation</t>
+  </si>
+  <si>
+    <t>source_active.xlsm</t>
+  </si>
+  <si>
+    <t>rgd_originel_completee_modifiee.xlsm"</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>Actions à mener:</t>
+  </si>
+  <si>
+    <t>F_lexique_batrub</t>
+  </si>
+  <si>
+    <t>Conversion en table</t>
+  </si>
+  <si>
+    <t>t_definition_cles_repartitions</t>
+  </si>
+  <si>
+    <t>t_lexique_bat</t>
+  </si>
+  <si>
+    <t>t_lexique_rub</t>
+  </si>
+  <si>
+    <t>t_lexique_typ</t>
+  </si>
+  <si>
+    <t>t_lexique_batrub</t>
+  </si>
+  <si>
+    <t>t_liste_groupes</t>
+  </si>
+  <si>
+    <t>t_liste_groupes_a_etudier</t>
+  </si>
+  <si>
+    <t>t_roc_modifiee</t>
+  </si>
+  <si>
+    <t>t_parametres</t>
+  </si>
+  <si>
+    <t>t_agregation</t>
+  </si>
+  <si>
+    <t>t_lexique_cles</t>
+  </si>
+  <si>
+    <t>exercice</t>
+  </si>
+  <si>
+    <t>date_a</t>
+  </si>
+  <si>
+    <t>rang_doublon</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>t_data</t>
+  </si>
+  <si>
+    <t>Composantes cle</t>
+  </si>
+  <si>
+    <t>cle</t>
+  </si>
+  <si>
+    <t>tampon_data (extraction Excel)</t>
+  </si>
+  <si>
+    <t>tampon_data:</t>
+  </si>
+  <si>
+    <t>Recueille les données de la feuille Excel "data" de source_active.xlsm et rien d'autre</t>
+  </si>
+  <si>
+    <t>Recueille les données de la feuille Excel "F_parametres" de source_active.xlsm et rien d'autre</t>
+  </si>
+  <si>
+    <t>Recueille les données de:</t>
+  </si>
+  <si>
+    <t>tampon_data</t>
+  </si>
+  <si>
+    <t>Enchainement des étapes</t>
+  </si>
+  <si>
+    <t>1)</t>
+  </si>
+  <si>
+    <t>Reinitialiser_bdd</t>
+  </si>
+  <si>
+    <t>Efface toutes les tables</t>
+  </si>
+  <si>
+    <t>Depuis lexiques.xls crée  les tables associées à des feuilles dont le nom est du type F_xxxx</t>
+  </si>
+  <si>
+    <t>Depuis source_active.xlsm crée les tables tampon_data et tampon_parametres.</t>
+  </si>
+  <si>
+    <t>Depuis rgd_originel_completee_modifiee.xlsm crée les tables t_agregation et t_roc_modifiee</t>
+  </si>
+  <si>
+    <t>Principe du processus</t>
+  </si>
+  <si>
+    <t>Descriptif des tables</t>
+  </si>
+  <si>
+    <t>Tranformations à apporter aux tables pour les mettre en sitution de fonctionnement</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Valeurs Null</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>Normer bat,rub,typ</t>
+  </si>
+  <si>
+    <t>Ajouter colonnes</t>
+  </si>
+  <si>
+    <t>Met aux normes t_roc_modifiee puis calcule la colonne cle</t>
+  </si>
+  <si>
+    <t>A l'initalisation, dans t_roc_modifiee calcule la colonne cle et crée la table lexique_cles à partir des colonnes cle et</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> groupe puis créela table lexique_cles à partir des deux colonnes cle et groupe</t>
+  </si>
+  <si>
+    <t>Copie les données de tampon_data et t_agregation dans t_data</t>
+  </si>
+  <si>
+    <t>Crée t_data à partir de son modèle</t>
+  </si>
+  <si>
+    <t>t_parametres:</t>
+  </si>
 </sst>
 </file>
 
@@ -2240,7 +2430,7 @@
     <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="166" formatCode="d/m/yy;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2320,8 +2510,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2352,6 +2549,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2362,7 +2565,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -2370,8 +2573,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2436,9 +2640,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 3" xfId="7" xr:uid="{09BF682D-1680-4330-9BD1-3044A6D81A95}"/>
     <cellStyle name="Normal_Feuil3" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal_Feuil4" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal_Feuil5" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
@@ -3449,6 +3661,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC9D70F-0DD0-4852-8227-16C3CCD3CB80}">
+  <sheetPr codeName="Feuil10"/>
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3531,6 +3744,846 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D103D7-A6CB-4FF3-BFE3-D1C6BF893BFB}">
+  <sheetPr codeName="Feuil11"/>
+  <dimension ref="A1:AF52"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1:X1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="2.84375" customWidth="1"/>
+    <col min="2" max="2" width="3.3046875" customWidth="1"/>
+    <col min="3" max="3" width="4.61328125" customWidth="1"/>
+    <col min="4" max="4" width="3.3046875" customWidth="1"/>
+    <col min="5" max="6" width="29.69140625" customWidth="1"/>
+    <col min="7" max="7" width="4.07421875" customWidth="1"/>
+    <col min="8" max="8" width="2.84375" customWidth="1"/>
+    <col min="9" max="9" width="2.765625" customWidth="1"/>
+    <col min="11" max="11" width="16.84375" customWidth="1"/>
+    <col min="12" max="12" width="1.3828125" style="32" customWidth="1"/>
+    <col min="13" max="13" width="2.3828125" customWidth="1"/>
+    <col min="14" max="14" width="21.15234375" customWidth="1"/>
+    <col min="15" max="15" width="2.61328125" customWidth="1"/>
+    <col min="16" max="16" width="17.53515625" customWidth="1"/>
+    <col min="17" max="17" width="14.921875" customWidth="1"/>
+    <col min="18" max="18" width="14.765625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.4609375" customWidth="1"/>
+    <col min="20" max="20" width="4.61328125" customWidth="1"/>
+    <col min="21" max="21" width="1.3828125" style="32" customWidth="1"/>
+    <col min="22" max="22" width="6.4609375" customWidth="1"/>
+    <col min="23" max="23" width="25.3828125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12" customWidth="1"/>
+    <col min="25" max="25" width="14.07421875" customWidth="1"/>
+    <col min="26" max="26" width="10.765625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.15234375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.69140625" customWidth="1"/>
+    <col min="30" max="30" width="16.4609375" customWidth="1"/>
+    <col min="31" max="31" width="13.3046875" customWidth="1"/>
+    <col min="32" max="32" width="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>491</v>
+      </c>
+      <c r="H1" t="s">
+        <v>502</v>
+      </c>
+      <c r="M1" t="s">
+        <v>541</v>
+      </c>
+      <c r="T1" s="1"/>
+      <c r="V1" s="31" t="s">
+        <v>542</v>
+      </c>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="B2" t="s">
+        <v>493</v>
+      </c>
+      <c r="T2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="C3" t="s">
+        <v>492</v>
+      </c>
+      <c r="F3" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="C4" t="s">
+        <v>494</v>
+      </c>
+      <c r="F4" t="s">
+        <v>510</v>
+      </c>
+      <c r="N4" s="30" t="s">
+        <v>527</v>
+      </c>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30" t="s">
+        <v>501</v>
+      </c>
+      <c r="Q4" s="30" t="s">
+        <v>498</v>
+      </c>
+      <c r="R4" s="30" t="s">
+        <v>525</v>
+      </c>
+      <c r="S4" s="30" t="s">
+        <v>524</v>
+      </c>
+      <c r="X4" s="30" t="s">
+        <v>543</v>
+      </c>
+      <c r="Y4" s="30" t="s">
+        <v>545</v>
+      </c>
+      <c r="Z4" s="30" t="s">
+        <v>544</v>
+      </c>
+      <c r="AA4" s="30" t="s">
+        <v>546</v>
+      </c>
+      <c r="AB4" s="30" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="C5" t="s">
+        <v>495</v>
+      </c>
+      <c r="F5" t="s">
+        <v>511</v>
+      </c>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" t="s">
+        <v>509</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="C6" t="s">
+        <v>499</v>
+      </c>
+      <c r="F6" t="s">
+        <v>512</v>
+      </c>
+      <c r="N6" t="s">
+        <v>413</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="31" t="s">
+        <v>412</v>
+      </c>
+      <c r="W6" t="s">
+        <v>510</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="C7" t="s">
+        <v>507</v>
+      </c>
+      <c r="F7" t="s">
+        <v>513</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="S7" s="31" t="s">
+        <v>520</v>
+      </c>
+      <c r="W7" t="s">
+        <v>511</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="C8" t="s">
+        <v>496</v>
+      </c>
+      <c r="F8" t="s">
+        <v>514</v>
+      </c>
+      <c r="N8" t="s">
+        <v>396</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="31"/>
+      <c r="W8" t="s">
+        <v>512</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="C9" t="s">
+        <v>497</v>
+      </c>
+      <c r="F9" t="s">
+        <v>515</v>
+      </c>
+      <c r="N9" t="s">
+        <v>406</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="R9" s="1"/>
+      <c r="S9" s="31" t="s">
+        <v>405</v>
+      </c>
+      <c r="W9" t="s">
+        <v>513</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="N10" t="s">
+        <v>404</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="S10" s="31" t="s">
+        <v>423</v>
+      </c>
+      <c r="W10" t="s">
+        <v>514</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="B11" t="s">
+        <v>504</v>
+      </c>
+      <c r="H11" t="s">
+        <v>503</v>
+      </c>
+      <c r="N11" t="s">
+        <v>403</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="31" t="s">
+        <v>417</v>
+      </c>
+      <c r="W11" t="s">
+        <v>515</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="AA11" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="C12" t="s">
+        <v>498</v>
+      </c>
+      <c r="F12" t="s">
+        <v>516</v>
+      </c>
+      <c r="I12" t="s">
+        <v>505</v>
+      </c>
+      <c r="N12" t="s">
+        <v>402</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="S12" s="31" t="s">
+        <v>424</v>
+      </c>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="C13" t="s">
+        <v>500</v>
+      </c>
+      <c r="F13" t="s">
+        <v>517</v>
+      </c>
+      <c r="I13" t="s">
+        <v>500</v>
+      </c>
+      <c r="N13" t="s">
+        <v>401</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="31" t="s">
+        <v>418</v>
+      </c>
+      <c r="W13" t="s">
+        <v>516</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="AA13" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="C14" t="s">
+        <v>501</v>
+      </c>
+      <c r="F14" t="s">
+        <v>518</v>
+      </c>
+      <c r="N14" t="s">
+        <v>400</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="S14" s="31" t="s">
+        <v>425</v>
+      </c>
+      <c r="W14" t="s">
+        <v>517</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="N15" t="s">
+        <v>399</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="R15" s="1"/>
+      <c r="S15" s="31" t="s">
+        <v>419</v>
+      </c>
+      <c r="W15" t="s">
+        <v>518</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="Z15" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="AA15" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="F16" t="s">
+        <v>519</v>
+      </c>
+      <c r="N16" t="s">
+        <v>398</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="S16" s="31" t="s">
+        <v>521</v>
+      </c>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="N17" t="s">
+        <v>396</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="S17" s="31" t="s">
+        <v>395</v>
+      </c>
+      <c r="W17" t="s">
+        <v>519</v>
+      </c>
+      <c r="X17" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>506</v>
+      </c>
+      <c r="N18" t="s">
+        <v>394</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="S18" s="31" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B19" t="s">
+        <v>491</v>
+      </c>
+      <c r="N19" t="s">
+        <v>392</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="S19" s="31" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="C20" t="s">
+        <v>492</v>
+      </c>
+      <c r="F20" t="s">
+        <v>509</v>
+      </c>
+      <c r="G20" t="s">
+        <v>508</v>
+      </c>
+      <c r="N20" t="s">
+        <v>391</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="S20" s="31" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="C21" t="s">
+        <v>494</v>
+      </c>
+      <c r="F21" t="s">
+        <v>510</v>
+      </c>
+      <c r="G21" t="s">
+        <v>508</v>
+      </c>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="S21" s="31" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="C22" t="s">
+        <v>495</v>
+      </c>
+      <c r="F22" t="s">
+        <v>511</v>
+      </c>
+      <c r="G22" t="s">
+        <v>508</v>
+      </c>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="R22" s="1"/>
+      <c r="S22" s="31" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="C23" t="s">
+        <v>499</v>
+      </c>
+      <c r="F23" t="s">
+        <v>512</v>
+      </c>
+      <c r="G23" t="s">
+        <v>508</v>
+      </c>
+      <c r="N23" t="s">
+        <v>410</v>
+      </c>
+      <c r="S23" s="31" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="C24" t="s">
+        <v>507</v>
+      </c>
+      <c r="F24" t="s">
+        <v>513</v>
+      </c>
+      <c r="G24" t="s">
+        <v>508</v>
+      </c>
+      <c r="N24" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="C25" t="s">
+        <v>496</v>
+      </c>
+      <c r="F25" t="s">
+        <v>514</v>
+      </c>
+      <c r="G25" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="C26" t="s">
+        <v>497</v>
+      </c>
+      <c r="F26" t="s">
+        <v>515</v>
+      </c>
+      <c r="G26" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="C28" t="s">
+        <v>498</v>
+      </c>
+      <c r="F28" t="s">
+        <v>516</v>
+      </c>
+      <c r="G28" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="C29" t="s">
+        <v>500</v>
+      </c>
+      <c r="F29" t="s">
+        <v>517</v>
+      </c>
+      <c r="G29" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="C30" t="s">
+        <v>501</v>
+      </c>
+      <c r="F30" t="s">
+        <v>518</v>
+      </c>
+      <c r="G30" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="B32" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C33" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B34" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C35" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B36" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C37" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D38" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D39" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="B42" t="s">
+        <v>534</v>
+      </c>
+      <c r="C42" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C43" s="31">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D43" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C44" s="31">
+        <v>1.2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C45" s="31">
+        <v>1.3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C46" s="31">
+        <v>1.4</v>
+      </c>
+      <c r="D46" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C47" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="D47" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C48" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.4">
+      <c r="D49" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="50" spans="4:5" x14ac:dyDescent="0.4">
+      <c r="D50" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.4">
+      <c r="E51" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="52" spans="4:5" x14ac:dyDescent="0.4">
+      <c r="D52" t="s">
+        <v>551</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -6508,7 +7561,7 @@
   <sheetPr codeName="Feuil7"/>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
@@ -6967,6 +8020,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46DB1BB2-6ACE-438E-8C42-3EC7DFCD420B}">
+  <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">

</xml_diff>

<commit_message>
Le module reinitialiser_bdd modifié pour la 3ème fois après avoir constaté que la coexistence de modeles et d'un fonctionnement à partir de requetes pures SQLITE3 pose problème.
</commit_message>
<xml_diff>
--- a/sources/lexiques.xlsx
+++ b/sources/lexiques.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Yvon\AAAAA-Mes-donnees\Mes-developpements\Python_tous_mes_tutoriels\projet_rgd_pas_a_pas\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B611D0F4-7DF4-4C3B-AD43-BC4CB0495122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6127880F-B729-4220-B22C-E3ADC926EBD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="564">
   <si>
     <t>E</t>
   </si>
@@ -2331,9 +2331,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>t_data</t>
-  </si>
-  <si>
     <t>Composantes cle</t>
   </si>
   <si>
@@ -2367,9 +2364,6 @@
     <t>Reinitialiser_bdd</t>
   </si>
   <si>
-    <t>Efface toutes les tables</t>
-  </si>
-  <si>
     <t>Depuis lexiques.xls crée  les tables associées à des feuilles dont le nom est du type F_xxxx</t>
   </si>
   <si>
@@ -2412,13 +2406,49 @@
     <t xml:space="preserve"> groupe puis créela table lexique_cles à partir des deux colonnes cle et groupe</t>
   </si>
   <si>
-    <t>Copie les données de tampon_data et t_agregation dans t_data</t>
-  </si>
-  <si>
-    <t>Crée t_data à partir de son modèle</t>
-  </si>
-  <si>
     <t>t_parametres:</t>
+  </si>
+  <si>
+    <t>2)</t>
+  </si>
+  <si>
+    <t>Actualiser les données</t>
+  </si>
+  <si>
+    <t>t_base_data</t>
+  </si>
+  <si>
+    <t>Crée t_base_data à partir de son modèle</t>
+  </si>
+  <si>
+    <t>Copie dans t_base_data les données de t_agregation et t_roc_modifiee</t>
+  </si>
+  <si>
+    <t>Renomme t_base_data en t_base_data_old</t>
+  </si>
+  <si>
+    <t>2.2)</t>
+  </si>
+  <si>
+    <t>Depuis source_active.xlsm crée les tables tampon_data et t_parametres.</t>
+  </si>
+  <si>
+    <t>2.3)</t>
+  </si>
+  <si>
+    <t>Norme tampon_data sur les noms de colonnes, les types, les valeurs Null, PK, les valeurs bat,rub,typ.</t>
+  </si>
+  <si>
+    <t>Efface toutes les tables de la liste ["t_roc_modifiee"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efface toutes les tables </t>
+  </si>
+  <si>
+    <t>2.4)</t>
+  </si>
+  <si>
+    <t>Noms colonnes</t>
   </si>
 </sst>
 </file>
@@ -3750,10 +3780,10 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D103D7-A6CB-4FF3-BFE3-D1C6BF893BFB}">
   <sheetPr codeName="Feuil11"/>
-  <dimension ref="A1:AF52"/>
+  <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:X1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3779,18 +3809,19 @@
     <col min="21" max="21" width="1.3828125" style="32" customWidth="1"/>
     <col min="22" max="22" width="6.4609375" customWidth="1"/>
     <col min="23" max="23" width="25.3828125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12" customWidth="1"/>
-    <col min="25" max="25" width="14.07421875" customWidth="1"/>
-    <col min="26" max="26" width="10.765625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.15234375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.69140625" customWidth="1"/>
-    <col min="30" max="30" width="16.4609375" customWidth="1"/>
-    <col min="31" max="31" width="13.3046875" customWidth="1"/>
-    <col min="32" max="32" width="8" customWidth="1"/>
+    <col min="24" max="24" width="13.3046875" customWidth="1"/>
+    <col min="25" max="25" width="12" customWidth="1"/>
+    <col min="26" max="26" width="14.07421875" customWidth="1"/>
+    <col min="27" max="27" width="10.765625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.15234375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.69140625" customWidth="1"/>
+    <col min="31" max="31" width="16.4609375" customWidth="1"/>
+    <col min="32" max="32" width="13.3046875" customWidth="1"/>
+    <col min="33" max="33" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>491</v>
       </c>
@@ -3798,11 +3829,11 @@
         <v>502</v>
       </c>
       <c r="M1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="T1" s="1"/>
       <c r="V1" s="31" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
@@ -3814,8 +3845,9 @@
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="AG1" s="1"/>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>493</v>
       </c>
@@ -3831,8 +3863,9 @@
       <c r="AD2" s="1"/>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="AG2" s="1"/>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.4">
       <c r="C3" t="s">
         <v>492</v>
       </c>
@@ -3840,7 +3873,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.4">
       <c r="C4" t="s">
         <v>494</v>
       </c>
@@ -3848,7 +3881,7 @@
         <v>510</v>
       </c>
       <c r="N4" s="30" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="O4" s="30"/>
       <c r="P4" s="30" t="s">
@@ -3858,28 +3891,31 @@
         <v>498</v>
       </c>
       <c r="R4" s="30" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="S4" s="30" t="s">
-        <v>524</v>
+        <v>552</v>
       </c>
       <c r="X4" s="30" t="s">
+        <v>563</v>
+      </c>
+      <c r="Y4" s="30" t="s">
+        <v>541</v>
+      </c>
+      <c r="Z4" s="30" t="s">
         <v>543</v>
       </c>
-      <c r="Y4" s="30" t="s">
+      <c r="AA4" s="30" t="s">
+        <v>542</v>
+      </c>
+      <c r="AB4" s="30" t="s">
+        <v>544</v>
+      </c>
+      <c r="AC4" s="30" t="s">
         <v>545</v>
       </c>
-      <c r="Z4" s="30" t="s">
-        <v>544</v>
-      </c>
-      <c r="AA4" s="30" t="s">
-        <v>546</v>
-      </c>
-      <c r="AB4" s="30" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.4">
       <c r="C5" t="s">
         <v>495</v>
       </c>
@@ -3892,23 +3928,23 @@
       <c r="W5" t="s">
         <v>509</v>
       </c>
-      <c r="X5" s="1" t="s">
-        <v>523</v>
-      </c>
       <c r="Y5" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1" t="s">
+      <c r="Z5" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AB5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1" t="s">
+        <v>523</v>
+      </c>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="AG5" s="1"/>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.4">
       <c r="C6" t="s">
         <v>499</v>
       </c>
@@ -3929,17 +3965,17 @@
       <c r="W6" t="s">
         <v>510</v>
       </c>
-      <c r="X6" s="1" t="s">
-        <v>523</v>
-      </c>
       <c r="Y6" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AA6" s="1" t="s">
+      <c r="Z6" s="1" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="AB6" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.4">
       <c r="C7" t="s">
         <v>507</v>
       </c>
@@ -3961,17 +3997,17 @@
       <c r="W7" t="s">
         <v>511</v>
       </c>
-      <c r="X7" s="1" t="s">
-        <v>523</v>
-      </c>
       <c r="Y7" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AA7" s="1" t="s">
+      <c r="Z7" s="1" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="AB7" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.4">
       <c r="C8" t="s">
         <v>496</v>
       </c>
@@ -3990,17 +4026,17 @@
       <c r="W8" t="s">
         <v>512</v>
       </c>
-      <c r="X8" s="1" t="s">
-        <v>523</v>
-      </c>
       <c r="Y8" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AA8" s="1" t="s">
+      <c r="Z8" s="1" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="AB8" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.4">
       <c r="C9" t="s">
         <v>497</v>
       </c>
@@ -4023,17 +4059,17 @@
       <c r="W9" t="s">
         <v>513</v>
       </c>
-      <c r="X9" s="1" t="s">
-        <v>523</v>
-      </c>
       <c r="Y9" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AA9" s="1" t="s">
+      <c r="Z9" s="1" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="AB9" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.4">
       <c r="N10" t="s">
         <v>404</v>
       </c>
@@ -4052,17 +4088,17 @@
       <c r="W10" t="s">
         <v>514</v>
       </c>
-      <c r="X10" s="1" t="s">
-        <v>523</v>
-      </c>
       <c r="Y10" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AA10" s="1" t="s">
+      <c r="Z10" s="1" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="AB10" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
         <v>504</v>
       </c>
@@ -4083,17 +4119,17 @@
       <c r="W11" t="s">
         <v>515</v>
       </c>
-      <c r="X11" s="1" t="s">
-        <v>523</v>
-      </c>
       <c r="Y11" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AA11" s="1" t="s">
+      <c r="Z11" s="1" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="AB11" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.4">
       <c r="C12" t="s">
         <v>498</v>
       </c>
@@ -4118,10 +4154,10 @@
       <c r="S12" s="31" t="s">
         <v>424</v>
       </c>
-      <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="Z12" s="1"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.4">
       <c r="C13" t="s">
         <v>500</v>
       </c>
@@ -4145,9 +4181,6 @@
       <c r="W13" t="s">
         <v>516</v>
       </c>
-      <c r="X13" s="1" t="s">
-        <v>523</v>
-      </c>
       <c r="Y13" s="1" t="s">
         <v>523</v>
       </c>
@@ -4157,8 +4190,11 @@
       <c r="AA13" s="1" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="AB13" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.4">
       <c r="C14" t="s">
         <v>501</v>
       </c>
@@ -4183,18 +4219,18 @@
       <c r="W14" t="s">
         <v>517</v>
       </c>
-      <c r="X14" s="1" t="s">
-        <v>523</v>
-      </c>
       <c r="Y14" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="1" t="s">
+      <c r="Z14" s="1" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.4">
       <c r="N15" t="s">
         <v>399</v>
       </c>
@@ -4211,9 +4247,6 @@
       <c r="W15" t="s">
         <v>518</v>
       </c>
-      <c r="X15" s="1" t="s">
-        <v>523</v>
-      </c>
       <c r="Y15" s="1" t="s">
         <v>523</v>
       </c>
@@ -4223,8 +4256,11 @@
       <c r="AA15" s="1" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.4">
+      <c r="AB15" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.4">
       <c r="F16" t="s">
         <v>519</v>
       </c>
@@ -4243,10 +4279,26 @@
       <c r="S16" s="31" t="s">
         <v>521</v>
       </c>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="W16" t="s">
+        <v>531</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="Z16" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="AA16" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="AB16" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.4">
       <c r="N17" t="s">
         <v>396</v>
       </c>
@@ -4262,17 +4314,8 @@
       <c r="S17" s="31" t="s">
         <v>395</v>
       </c>
-      <c r="W17" t="s">
-        <v>519</v>
-      </c>
-      <c r="X17" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="Y17" s="1" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.4">
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>506</v>
       </c>
@@ -4291,8 +4334,17 @@
       <c r="S18" s="31" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.4">
+      <c r="W18" t="s">
+        <v>519</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="Z18" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
         <v>491</v>
       </c>
@@ -4312,7 +4364,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.4">
       <c r="C20" t="s">
         <v>492</v>
       </c>
@@ -4338,7 +4390,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.4">
       <c r="C21" t="s">
         <v>494</v>
       </c>
@@ -4359,7 +4411,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.4">
       <c r="C22" t="s">
         <v>495</v>
       </c>
@@ -4378,7 +4430,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.4">
       <c r="C23" t="s">
         <v>499</v>
       </c>
@@ -4392,10 +4444,10 @@
         <v>410</v>
       </c>
       <c r="S23" s="31" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.4">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.4">
       <c r="C24" t="s">
         <v>507</v>
       </c>
@@ -4409,7 +4461,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.4">
       <c r="C25" t="s">
         <v>496</v>
       </c>
@@ -4420,7 +4472,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.4">
       <c r="C26" t="s">
         <v>497</v>
       </c>
@@ -4431,7 +4483,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.4">
       <c r="C28" t="s">
         <v>498</v>
       </c>
@@ -4442,7 +4494,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.4">
       <c r="C29" t="s">
         <v>500</v>
       </c>
@@ -4453,7 +4505,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.4">
       <c r="C30" t="s">
         <v>501</v>
       </c>
@@ -4464,34 +4516,34 @@
         <v>508</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C33" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B34" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C35" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
-        <v>524</v>
+        <v>552</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C37" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.4">
@@ -4501,20 +4553,20 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.4">
       <c r="D39" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
+        <v>533</v>
+      </c>
+      <c r="C42" t="s">
         <v>534</v>
-      </c>
-      <c r="C42" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.4">
@@ -4522,7 +4574,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="D43" t="s">
-        <v>536</v>
+        <v>561</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.4">
@@ -4530,7 +4582,7 @@
         <v>1.2</v>
       </c>
       <c r="D44" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.4">
@@ -4538,7 +4590,7 @@
         <v>1.3</v>
       </c>
       <c r="D45" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.4">
@@ -4546,7 +4598,7 @@
         <v>1.4</v>
       </c>
       <c r="D46" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.4">
@@ -4554,36 +4606,80 @@
         <v>1.5</v>
       </c>
       <c r="D47" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="C48" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.4">
-      <c r="D49" t="s">
+      <c r="C48" s="31">
+        <v>1.6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C49" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="D50" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="D51" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="E52" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="50" spans="4:5" x14ac:dyDescent="0.4">
-      <c r="D50" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.4">
-      <c r="E51" t="s">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B53" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="52" spans="4:5" x14ac:dyDescent="0.4">
-      <c r="D52" t="s">
+      <c r="C53" t="s">
         <v>551</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C54" s="31">
+        <v>2.1</v>
+      </c>
+      <c r="D54" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C55" t="s">
+        <v>556</v>
+      </c>
+      <c r="D55" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C56" t="s">
+        <v>558</v>
+      </c>
+      <c r="D56" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="C57" t="s">
+        <v>562</v>
+      </c>
+      <c r="D57" t="s">
+        <v>559</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Nouvelle structure: Centralisation des variables communes
</commit_message>
<xml_diff>
--- a/sources/lexiques.xlsx
+++ b/sources/lexiques.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Yvon\AAAAA-Mes-donnees\Mes-developpements\Python_tous_mes_tutoriels\projet_rgd_pas_a_pas\sources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mes_dossiers_synchronises\projet_rgd_pas_a_pas\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6127880F-B729-4220-B22C-E3ADC926EBD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D449DF0E-F720-4CA2-B015-80FE1B83DD54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F_definition_cles_repartitions" sheetId="2" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="Règles de nommage (PEP8)" sheetId="11" r:id="rId9"/>
     <sheet name="Classe vs Table" sheetId="12" r:id="rId10"/>
     <sheet name="Processus" sheetId="13" r:id="rId11"/>
+    <sheet name="Enchainements" sheetId="14" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="Agregation_2015_a_2019">#REF!</definedName>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="599">
   <si>
     <t>E</t>
   </si>
@@ -2450,6 +2451,111 @@
   <si>
     <t>Noms colonnes</t>
   </si>
+  <si>
+    <t>main.py</t>
+  </si>
+  <si>
+    <t>from src.core.context import app_context</t>
+  </si>
+  <si>
+    <t>MODE_DEBUG</t>
+  </si>
+  <si>
+    <t>VERSION</t>
+  </si>
+  <si>
+    <t>NOM_APPLICATION</t>
+  </si>
+  <si>
+    <t>NOM_COURT</t>
+  </si>
+  <si>
+    <t>PALETTES</t>
+  </si>
+  <si>
+    <t>POLICES</t>
+  </si>
+  <si>
+    <t>rep_bdd</t>
+  </si>
+  <si>
+    <t>db</t>
+  </si>
+  <si>
+    <t>mode_debug</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>nom_application</t>
+  </si>
+  <si>
+    <t>nom_court</t>
+  </si>
+  <si>
+    <t>palettes</t>
+  </si>
+  <si>
+    <t>polices</t>
+  </si>
+  <si>
+    <t>paths.rep_defaut</t>
+  </si>
+  <si>
+    <t>paths.rep_source</t>
+  </si>
+  <si>
+    <t>paths.rep_resultats</t>
+  </si>
+  <si>
+    <t>paths.rep_data</t>
+  </si>
+  <si>
+    <t>Ne doivent pas être utilisés hors context.py</t>
+  </si>
+  <si>
+    <t>POLICE</t>
+  </si>
+  <si>
+    <t>police</t>
+  </si>
+  <si>
+    <t>palette</t>
+  </si>
+  <si>
+    <t>PALETTE</t>
+  </si>
+  <si>
+    <t>Les fichiers générateurs des variables produites par context.py</t>
+  </si>
+  <si>
+    <t>parametres.py</t>
+  </si>
+  <si>
+    <t>variables_metier_path.py</t>
+  </si>
+  <si>
+    <t>engine</t>
+  </si>
+  <si>
+    <t>ENGINE</t>
+  </si>
+  <si>
+    <t>Dans tous les autres modules, les variables de path (yc. ENGINE) et parametres doivent être accédées par from context import context</t>
+  </si>
+  <si>
+    <t>variables_metier.py</t>
+  </si>
+  <si>
+    <t>Accès autorisés aux variable communes:</t>
+  </si>
+  <si>
+    <t>from src.core.context import context as ctxt</t>
+  </si>
+  <si>
+    <t>from src.core.variables_metier as vm</t>
+  </si>
 </sst>
 </file>
 
@@ -2460,7 +2566,7 @@
     <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
     <numFmt numFmtId="166" formatCode="d/m/yy;@"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2547,8 +2653,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2585,6 +2702,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2605,7 +2734,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2677,6 +2806,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3782,7 +3923,7 @@
   <sheetPr codeName="Feuil11"/>
   <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
@@ -4683,6 +4824,260 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69CBAFF4-08AC-491E-AD67-76A1294D9969}">
+  <dimension ref="A1:M20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="2" width="3.3828125" customWidth="1"/>
+    <col min="3" max="3" width="31.53515625" customWidth="1"/>
+    <col min="4" max="4" width="3.3828125" customWidth="1"/>
+    <col min="5" max="5" width="2.07421875" style="32" customWidth="1"/>
+    <col min="6" max="6" width="2.69140625" customWidth="1"/>
+    <col min="7" max="7" width="34.3828125" customWidth="1"/>
+    <col min="8" max="8" width="2.921875" customWidth="1"/>
+    <col min="9" max="9" width="2.07421875" style="32" customWidth="1"/>
+    <col min="10" max="10" width="3.23046875" customWidth="1"/>
+    <col min="11" max="11" width="3.765625" customWidth="1"/>
+    <col min="13" max="13" width="26.23046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>564</v>
+      </c>
+      <c r="F1" t="s">
+        <v>584</v>
+      </c>
+      <c r="J1" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B2" t="s">
+        <v>565</v>
+      </c>
+      <c r="G2" t="s">
+        <v>570</v>
+      </c>
+      <c r="K2" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C3" s="33" t="s">
+        <v>574</v>
+      </c>
+      <c r="D3" s="34"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="34"/>
+      <c r="G3" t="s">
+        <v>571</v>
+      </c>
+      <c r="I3" s="37"/>
+      <c r="K3" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C4" s="33" t="s">
+        <v>575</v>
+      </c>
+      <c r="D4" s="34"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="34"/>
+      <c r="G4" t="s">
+        <v>566</v>
+      </c>
+      <c r="I4" s="37"/>
+      <c r="K4" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C5" s="33" t="s">
+        <v>576</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="34"/>
+      <c r="G5" t="s">
+        <v>567</v>
+      </c>
+      <c r="I5" s="37"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C6" s="33" t="s">
+        <v>577</v>
+      </c>
+      <c r="D6" s="34"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="34"/>
+      <c r="G6" t="s">
+        <v>568</v>
+      </c>
+      <c r="I6" s="37"/>
+      <c r="J6" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C7" s="33" t="s">
+        <v>578</v>
+      </c>
+      <c r="D7" s="34"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="34"/>
+      <c r="G7" t="s">
+        <v>569</v>
+      </c>
+      <c r="I7" s="37"/>
+      <c r="K7" s="38" t="s">
+        <v>596</v>
+      </c>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C8" s="33" t="s">
+        <v>579</v>
+      </c>
+      <c r="D8" s="34"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="34"/>
+      <c r="G8" t="s">
+        <v>588</v>
+      </c>
+      <c r="I8" s="37"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38" t="s">
+        <v>597</v>
+      </c>
+      <c r="M8" s="38"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C9" s="33" t="s">
+        <v>587</v>
+      </c>
+      <c r="D9" s="34"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="34"/>
+      <c r="G9" t="s">
+        <v>585</v>
+      </c>
+      <c r="I9" s="37"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38" t="s">
+        <v>598</v>
+      </c>
+      <c r="M9" s="38"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C10" s="33" t="s">
+        <v>586</v>
+      </c>
+      <c r="D10" s="34"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="34"/>
+      <c r="G10" t="s">
+        <v>593</v>
+      </c>
+      <c r="I10" s="37"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C11" s="33" t="s">
+        <v>580</v>
+      </c>
+      <c r="D11" s="34"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="34"/>
+      <c r="I11" s="37"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C12" s="33" t="s">
+        <v>581</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="34"/>
+      <c r="I12" s="37"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C13" s="33" t="s">
+        <v>582</v>
+      </c>
+      <c r="D13" s="34"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="34"/>
+      <c r="I13" s="37"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C14" s="33" t="s">
+        <v>583</v>
+      </c>
+      <c r="D14" s="34"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="34"/>
+      <c r="I14" s="37"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C15" s="33" t="s">
+        <v>572</v>
+      </c>
+      <c r="D15" s="34"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="34"/>
+      <c r="I15" s="37"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C16" s="33" t="s">
+        <v>573</v>
+      </c>
+      <c r="D16" s="34"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="34"/>
+      <c r="I16" s="37"/>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.4">
+      <c r="C17" s="35" t="s">
+        <v>592</v>
+      </c>
+      <c r="D17" s="34"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="34"/>
+      <c r="I17" s="37"/>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.4">
+      <c r="C18" s="36"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="34"/>
+      <c r="I18" s="37"/>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.4">
+      <c r="C19" s="35"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="34"/>
+      <c r="I19" s="37"/>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.4">
+      <c r="C20" s="35"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="34"/>
+      <c r="I20" s="37"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Feuil2"/>

</xml_diff>

<commit_message>
Nouvelle structure: Integration des variables métier dans context. Présence d'une référence circulaire
</commit_message>
<xml_diff>
--- a/sources/lexiques.xlsx
+++ b/sources/lexiques.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mes_dossiers_synchronises\projet_rgd_pas_a_pas\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D449DF0E-F720-4CA2-B015-80FE1B83DD54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABA6FA4-12AB-4598-BD65-71F14408F96A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" firstSheet="2" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2548,13 +2548,13 @@
     <t>variables_metier.py</t>
   </si>
   <si>
-    <t>Accès autorisés aux variable communes:</t>
-  </si>
-  <si>
     <t>from src.core.context import context as ctxt</t>
   </si>
   <si>
     <t>from src.core.variables_metier as vm</t>
+  </si>
+  <si>
+    <t>Accès aux variable communes autorisés:</t>
   </si>
 </sst>
 </file>
@@ -4829,7 +4829,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4938,7 +4938,7 @@
       </c>
       <c r="I7" s="37"/>
       <c r="K7" s="38" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="L7" s="38"/>
       <c r="M7" s="38"/>
@@ -4956,7 +4956,7 @@
       <c r="I8" s="37"/>
       <c r="K8" s="38"/>
       <c r="L8" s="38" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="M8" s="38"/>
     </row>
@@ -4973,7 +4973,7 @@
       <c r="I9" s="37"/>
       <c r="K9" s="38"/>
       <c r="L9" s="38" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="M9" s="38"/>
     </row>

</xml_diff>